<commit_message>
Adjust filter in LED space heating to exclude space heating CGs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CAB61C-1D87-4E0A-9976-4B8B94FEE4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3039023-D63C-4F9A-8AFA-48988455366B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="218">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -883,6 +883,18 @@
   </si>
   <si>
     <t>Original value (2021)</t>
+  </si>
+  <si>
+    <t>RSDSH_Apt*-*</t>
+  </si>
+  <si>
+    <t>RSDSH_Att*-*</t>
+  </si>
+  <si>
+    <t>RSDSH_Det*-*</t>
+  </si>
+  <si>
+    <t>Top_check</t>
   </si>
 </sst>
 </file>
@@ -14493,7 +14505,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:AN42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
@@ -14590,7 +14602,7 @@
         <v>1.7028384806625201</v>
       </c>
       <c r="L3" s="30">
-        <f>K3*2/3+N3/3</f>
+        <f t="shared" ref="L3:L16" si="0">K3*2/3+N3/3</f>
         <v>1.1584060685789734</v>
       </c>
       <c r="N3" s="30">
@@ -14631,7 +14643,7 @@
         <v>23.738094411807602</v>
       </c>
       <c r="L4" s="30">
-        <f>K4*2/3+N4/3</f>
+        <f t="shared" si="0"/>
         <v>22.05783877515594</v>
       </c>
       <c r="N4" s="30">
@@ -14672,7 +14684,7 @@
         <v>1.5478463345837199</v>
       </c>
       <c r="L5" s="30">
-        <f>K5*2/3+N5/3</f>
+        <f t="shared" si="0"/>
         <v>1.9434753073389506</v>
       </c>
       <c r="N5" s="30">
@@ -14713,7 +14725,7 @@
         <v>5.8166390635502099</v>
       </c>
       <c r="L6" s="30">
-        <f>K6*2/3+N6/3</f>
+        <f t="shared" si="0"/>
         <v>5.2807562869892761</v>
       </c>
       <c r="N6" s="30">
@@ -14754,7 +14766,7 @@
         <v>1.19927927754182</v>
       </c>
       <c r="L7" s="30">
-        <f>K7*2/3+N7/3</f>
+        <f t="shared" si="0"/>
         <v>1.22325956804396</v>
       </c>
       <c r="N7" s="30">
@@ -14795,7 +14807,7 @@
         <v>10.6043548094603</v>
       </c>
       <c r="L8" s="30">
-        <f>K8*2/3+N8/3</f>
+        <f t="shared" si="0"/>
         <v>9.4725222533350699</v>
       </c>
       <c r="N8" s="30">
@@ -14836,7 +14848,7 @@
         <v>1.0410295169864401</v>
       </c>
       <c r="L9" s="30">
-        <f>K9*2/3+N9/3</f>
+        <f t="shared" si="0"/>
         <v>0.85675812345956381</v>
       </c>
       <c r="N9" s="30">
@@ -14877,7 +14889,7 @@
         <v>18.752348682008719</v>
       </c>
       <c r="L10" s="30">
-        <f>K10*2/3+N10/3</f>
+        <f t="shared" si="0"/>
         <v>15.463248848798345</v>
       </c>
       <c r="N10" s="30">
@@ -14918,7 +14930,7 @@
         <v>18.095637208589601</v>
       </c>
       <c r="L11" s="30">
-        <f>K11*2/3+N11/3</f>
+        <f t="shared" si="0"/>
         <v>16.048363755990756</v>
       </c>
       <c r="N11" s="30">
@@ -14959,7 +14971,7 @@
         <v>2.2584342466232901</v>
       </c>
       <c r="L12" s="30">
-        <f>K12*2/3+N12/3</f>
+        <f t="shared" si="0"/>
         <v>1.8148484316492632</v>
       </c>
       <c r="N12" s="30">
@@ -15000,7 +15012,7 @@
         <v>6.2862087424890802</v>
       </c>
       <c r="L13" s="30">
-        <f>K13*2/3+N13/3</f>
+        <f t="shared" si="0"/>
         <v>7.1919298250215675</v>
       </c>
       <c r="N13" s="30">
@@ -15041,7 +15053,7 @@
         <v>0.187409320968947</v>
       </c>
       <c r="L14" s="30">
-        <f>K14*2/3+N14/3</f>
+        <f t="shared" si="0"/>
         <v>0.1326581724749025</v>
       </c>
       <c r="N14" s="30">
@@ -15082,7 +15094,7 @@
         <v>4.6924479738735299</v>
       </c>
       <c r="L15" s="30">
-        <f>K15*2/3+N15/3</f>
+        <f t="shared" si="0"/>
         <v>4.2494582874450408</v>
       </c>
       <c r="N15" s="30">
@@ -15123,7 +15135,7 @@
         <v>3.6347440465271599</v>
       </c>
       <c r="L16" s="30">
-        <f>K16*2/3+N16/3</f>
+        <f t="shared" si="0"/>
         <v>3.5045513913327135</v>
       </c>
       <c r="N16" s="30">
@@ -15328,7 +15340,7 @@
         <v>8.6157094085103783</v>
       </c>
       <c r="K21" s="30">
-        <f t="shared" ref="K21" si="0">J21-($H$21/11)</f>
+        <f t="shared" ref="K21" si="1">J21-($H$21/11)</f>
         <v>7.6814227047944605</v>
       </c>
       <c r="L21" s="30">
@@ -16209,8 +16221,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="C4:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16218,6 +16230,7 @@
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16259,7 +16272,7 @@
         <v>148</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
@@ -16296,10 +16309,13 @@
         <v>200</v>
       </c>
       <c r="J7" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="K7" t="s">
         <v>155</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
@@ -16319,10 +16335,13 @@
         <v>201</v>
       </c>
       <c r="J8" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="K8" t="s">
         <v>155</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
@@ -16342,10 +16361,13 @@
         <v>202</v>
       </c>
       <c r="J9" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="K9" t="s">
         <v>155</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
@@ -16373,6 +16395,9 @@
       <c r="K10" t="s">
         <v>155</v>
       </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
@@ -16399,6 +16424,9 @@
       <c r="K11" t="s">
         <v>155</v>
       </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
@@ -16425,6 +16453,9 @@
       <c r="K12" t="s">
         <v>155</v>
       </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
@@ -16448,6 +16479,9 @@
       <c r="K13" t="s">
         <v>155</v>
       </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
@@ -16471,6 +16505,9 @@
       <c r="K14" t="s">
         <v>155</v>
       </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
@@ -16494,6 +16531,9 @@
       <c r="K15" t="s">
         <v>155</v>
       </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
@@ -16517,8 +16557,11 @@
       <c r="K16" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>151</v>
       </c>
@@ -16540,8 +16583,11 @@
       <c r="K17" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>151</v>
       </c>
@@ -16563,8 +16609,11 @@
       <c r="K18" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>151</v>
       </c>
@@ -16586,8 +16635,11 @@
       <c r="K19" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>151</v>
       </c>
@@ -16609,8 +16661,11 @@
       <c r="K20" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>151</v>
       </c>
@@ -16632,8 +16687,11 @@
       <c r="K21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>151</v>
       </c>
@@ -16650,13 +16708,16 @@
         <v>200</v>
       </c>
       <c r="J22" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="K22" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>151</v>
       </c>
@@ -16673,13 +16734,16 @@
         <v>201</v>
       </c>
       <c r="J23" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="K23" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>151</v>
       </c>
@@ -16696,13 +16760,16 @@
         <v>202</v>
       </c>
       <c r="J24" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="K24" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>156</v>
       </c>
@@ -16727,8 +16794,11 @@
       <c r="K25" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>156</v>
       </c>
@@ -16753,8 +16823,11 @@
       <c r="K26" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>156</v>
       </c>
@@ -16779,8 +16852,11 @@
       <c r="K27" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>151</v>
       </c>
@@ -16802,8 +16878,11 @@
       <c r="K28" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>151</v>
       </c>
@@ -16825,8 +16904,11 @@
       <c r="K29" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>151</v>
       </c>
@@ -16848,8 +16930,11 @@
       <c r="K30" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>151</v>
       </c>
@@ -16871,8 +16956,11 @@
       <c r="K31" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>151</v>
       </c>
@@ -16894,8 +16982,11 @@
       <c r="K32" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>151</v>
       </c>
@@ -16917,8 +17008,11 @@
       <c r="K33" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>151</v>
       </c>
@@ -16940,8 +17034,11 @@
       <c r="K34" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>151</v>
       </c>
@@ -16963,8 +17060,11 @@
       <c r="K35" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>151</v>
       </c>
@@ -16986,8 +17086,11 @@
       <c r="K36" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>151</v>
       </c>
@@ -17004,13 +17107,16 @@
         <v>200</v>
       </c>
       <c r="J37" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="K37" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>151</v>
       </c>
@@ -17027,13 +17133,16 @@
         <v>201</v>
       </c>
       <c r="J38" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="K38" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>151</v>
       </c>
@@ -17050,13 +17159,16 @@
         <v>202</v>
       </c>
       <c r="J39" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="K39" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>151</v>
       </c>
@@ -17078,8 +17190,11 @@
       <c r="K40" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>151</v>
       </c>
@@ -17101,8 +17216,11 @@
       <c r="K41" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>151</v>
       </c>
@@ -17124,8 +17242,11 @@
       <c r="K42" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>151</v>
       </c>
@@ -17147,8 +17268,11 @@
       <c r="K43" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>151</v>
       </c>
@@ -17170,8 +17294,11 @@
       <c r="K44" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>151</v>
       </c>
@@ -17193,8 +17320,11 @@
       <c r="K45" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>151</v>
       </c>
@@ -17216,8 +17346,11 @@
       <c r="K46" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>151</v>
       </c>
@@ -17239,8 +17372,11 @@
       <c r="K47" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>151</v>
       </c>
@@ -17262,8 +17398,11 @@
       <c r="K48" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>151</v>
       </c>
@@ -17285,8 +17424,11 @@
       <c r="K49" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>151</v>
       </c>
@@ -17308,8 +17450,11 @@
       <c r="K50" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
         <v>151</v>
       </c>
@@ -17330,6 +17475,9 @@
       </c>
       <c r="K51" t="s">
         <v>154</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>